<commit_message>
Updated with field descriptions and mapping to SEPA spec
</commit_message>
<xml_diff>
--- a/SEPA W3C mapping.xlsx
+++ b/SEPA W3C mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saxon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saxon\OneDrive\Documents\GitHub\webpayments-methods-credit-transfer-direct-debit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5955,15 +5955,6 @@
     <t>PayeePaymentIdentification</t>
   </si>
   <si>
-    <t>PreferredExecutionDate, SelectedExecutionDate</t>
-  </si>
-  <si>
-    <t>OriginatorIdentificationCode</t>
-  </si>
-  <si>
-    <t>ReferencePartyIdentificationCode</t>
-  </si>
-  <si>
     <t>Reference to the reference party for reconciliation</t>
   </si>
   <si>
@@ -5976,12 +5967,6 @@
     <t>Derived from the IBAN</t>
   </si>
   <si>
-    <t>PayeeReferencePartyIdentificationCode</t>
-  </si>
-  <si>
-    <t>PayeeReferencePartyName</t>
-  </si>
-  <si>
     <t>PayeeIdentificationCode</t>
   </si>
   <si>
@@ -6118,6 +6103,21 @@
   </si>
   <si>
     <t>Default value of "EPAY" (ePayment) should be used by Payment App if this is not supplied by the merchant</t>
+  </si>
+  <si>
+    <t>SellerName</t>
+  </si>
+  <si>
+    <t>SellerIdentificationCode</t>
+  </si>
+  <si>
+    <t>SelectedProcessingDate</t>
+  </si>
+  <si>
+    <t>PayerIdentificationCode</t>
+  </si>
+  <si>
+    <t>BuyerIdentificationCode</t>
   </si>
 </sst>
 </file>
@@ -6153,7 +6153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -6180,6 +6180,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -29286,7 +29291,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A5" sqref="A5:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29300,16 +29305,16 @@
     <col min="7" max="7" width="5.54296875" style="8" customWidth="1"/>
     <col min="8" max="8" width="8.54296875" style="8" customWidth="1"/>
     <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="37.6328125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="25.08984375" style="8" customWidth="1"/>
     <col min="11" max="11" width="52.6328125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1390</v>
@@ -29324,16 +29329,16 @@
         <v>1392</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>1400</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>1027</v>
@@ -29341,10 +29346,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
       <c r="F2" t="s">
         <v>1394</v>
@@ -29358,10 +29363,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
       <c r="F3" t="s">
         <v>1394</v>
@@ -29372,10 +29377,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="F4" t="s">
         <v>1394</v>
@@ -29384,267 +29389,272 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>1434</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
+        <v>1394</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>1406</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="J7" s="11" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>1437</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>1461</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>1439</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E10" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="K5" t="s">
-        <v>1398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>1435</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>1440</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="J11" s="11" t="s">
+        <v>1401</v>
+      </c>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="I6" t="s">
-        <v>1402</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>1406</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="J12" s="11" t="s">
+        <v>1409</v>
+      </c>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>1443</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>1411</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
         <v>1419</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>1441</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B17" s="11" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>1407</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="J17" s="11" t="s">
+        <v>1458</v>
+      </c>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>1420</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>1442</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B18" s="11" t="s">
+        <v>1447</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>1404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>1443</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="J18" s="11" t="s">
+        <v>1408</v>
+      </c>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>1409</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>1444</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="H19" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>1408</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="J19" s="12" t="s">
+        <v>1454</v>
+      </c>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>1421</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>1445</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B20" s="11" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="J11" s="8" t="s">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>1422</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>1446</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="J12" s="8" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>1430</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>1447</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1394</v>
-      </c>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>1448</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="K14" t="s">
-        <v>1413</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>1423</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>1449</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="J15" s="8" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>1432</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>1450</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="J16" s="8" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>1424</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>1451</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="J17" s="8" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>1425</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>1452</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="J18" s="8" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>1433</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>1453</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G19"/>
-      <c r="H19" t="s">
-        <v>1394</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>1426</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>1454</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="J20" s="8" t="s">
-        <v>1460</v>
-      </c>
-      <c r="K20" t="s">
-        <v>1461</v>
+      <c r="J20" s="11" t="s">
+        <v>1455</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>1456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with field descriptions and mapping to SEPA spec (#16)
</commit_message>
<xml_diff>
--- a/SEPA W3C mapping.xlsx
+++ b/SEPA W3C mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saxon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saxon\OneDrive\Documents\GitHub\webpayments-methods-credit-transfer-direct-debit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5955,15 +5955,6 @@
     <t>PayeePaymentIdentification</t>
   </si>
   <si>
-    <t>PreferredExecutionDate, SelectedExecutionDate</t>
-  </si>
-  <si>
-    <t>OriginatorIdentificationCode</t>
-  </si>
-  <si>
-    <t>ReferencePartyIdentificationCode</t>
-  </si>
-  <si>
     <t>Reference to the reference party for reconciliation</t>
   </si>
   <si>
@@ -5976,12 +5967,6 @@
     <t>Derived from the IBAN</t>
   </si>
   <si>
-    <t>PayeeReferencePartyIdentificationCode</t>
-  </si>
-  <si>
-    <t>PayeeReferencePartyName</t>
-  </si>
-  <si>
     <t>PayeeIdentificationCode</t>
   </si>
   <si>
@@ -6118,6 +6103,21 @@
   </si>
   <si>
     <t>Default value of "EPAY" (ePayment) should be used by Payment App if this is not supplied by the merchant</t>
+  </si>
+  <si>
+    <t>SellerName</t>
+  </si>
+  <si>
+    <t>SellerIdentificationCode</t>
+  </si>
+  <si>
+    <t>SelectedProcessingDate</t>
+  </si>
+  <si>
+    <t>PayerIdentificationCode</t>
+  </si>
+  <si>
+    <t>BuyerIdentificationCode</t>
   </si>
 </sst>
 </file>
@@ -6153,7 +6153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -6180,6 +6180,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -29286,7 +29291,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A5" sqref="A5:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29300,16 +29305,16 @@
     <col min="7" max="7" width="5.54296875" style="8" customWidth="1"/>
     <col min="8" max="8" width="8.54296875" style="8" customWidth="1"/>
     <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="37.6328125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="25.08984375" style="8" customWidth="1"/>
     <col min="11" max="11" width="52.6328125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1390</v>
@@ -29324,16 +29329,16 @@
         <v>1392</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>1400</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>1027</v>
@@ -29341,10 +29346,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
       <c r="F2" t="s">
         <v>1394</v>
@@ -29358,10 +29363,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
       <c r="F3" t="s">
         <v>1394</v>
@@ -29372,10 +29377,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="F4" t="s">
         <v>1394</v>
@@ -29384,267 +29389,272 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>1434</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
+        <v>1394</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>1402</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>1406</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="J7" s="11" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>1437</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>1461</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>1439</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E10" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="K5" t="s">
-        <v>1398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>1435</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>1440</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="J11" s="11" t="s">
+        <v>1401</v>
+      </c>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="I6" t="s">
-        <v>1402</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>1406</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="J12" s="11" t="s">
+        <v>1409</v>
+      </c>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>1443</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>1411</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
         <v>1419</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>1441</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B17" s="11" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>1407</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="J17" s="11" t="s">
+        <v>1458</v>
+      </c>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>1420</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>1442</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B18" s="11" t="s">
+        <v>1447</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>1404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>1443</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="J18" s="11" t="s">
+        <v>1408</v>
+      </c>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>1409</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>1444</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="H19" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>1408</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="J19" s="12" t="s">
+        <v>1454</v>
+      </c>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>1421</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>1445</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B20" s="11" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>1394</v>
       </c>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="J11" s="8" t="s">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>1422</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>1446</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="J12" s="8" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>1430</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>1447</v>
-      </c>
-      <c r="G13" t="s">
-        <v>1394</v>
-      </c>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>1448</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="K14" t="s">
-        <v>1413</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>1423</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>1449</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="J15" s="8" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>1432</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>1450</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="J16" s="8" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>1424</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>1451</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="J17" s="8" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>1425</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>1452</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="J18" s="8" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>1433</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>1453</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G19"/>
-      <c r="H19" t="s">
-        <v>1394</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>1426</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>1454</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1394</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="J20" s="8" t="s">
-        <v>1460</v>
-      </c>
-      <c r="K20" t="s">
-        <v>1461</v>
+      <c r="J20" s="11" t="s">
+        <v>1455</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>1456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>